<commit_message>
UPDATED MULTcompare for diel period for lmb
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/diel-period/lmb/glmm_multi_comp_dp_LMB.xlsx
+++ b/results/accel-glmm-results/diel-period/lmb/glmm_multi_comp_dp_LMB.xlsx
@@ -1,76 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CU\Data\toronto-lmb-np-accel\results\accel-glmm-results\diel-period\lmb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D9EDB4-27E6-4D2C-B3D2-110AA2655B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t xml:space="preserve">term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contrast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">std_error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">statistic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adj_p_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">day_night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day / Night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dawn / Night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dusk / Night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dawn / Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dawn / Dusk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day / Dusk</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>contrast</t>
+  </si>
+  <si>
+    <t>null_value</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>std_error</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>adj_p_value</t>
+  </si>
+  <si>
+    <t>day_night</t>
+  </si>
+  <si>
+    <t>Day / Night</t>
+  </si>
+  <si>
+    <t>Dawn / Night</t>
+  </si>
+  <si>
+    <t>Dusk / Night</t>
+  </si>
+  <si>
+    <t>Dawn / Day</t>
+  </si>
+  <si>
+    <t>Dawn / Dusk</t>
+  </si>
+  <si>
+    <t>Day / Dusk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,13 +125,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -384,14 +424,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,182 +467,183 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>1.2261215482216</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.00937873218832941</v>
+      <c r="D2">
+        <v>1.2261215482215999</v>
+      </c>
+      <c r="E2">
+        <v>9.3787321883294101E-3</v>
       </c>
       <c r="F2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>26.6509586051659</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000104668930149481</v>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>26.650958605165901</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1.0466893014948101E-155</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>1.33295907500781</v>
       </c>
-      <c r="E3" t="n">
-        <v>0.0213047835317264</v>
+      <c r="E3">
+        <v>2.13047835317264E-2</v>
       </c>
       <c r="F3" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
         <v>17.9816060006684</v>
       </c>
-      <c r="I3" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000016290776717865</v>
+      <c r="I3" s="1">
+        <v>1.6290776717865001E-71</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>1.23856235686522</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.0215725621159794</v>
+      <c r="E4">
+        <v>2.15725621159794E-2</v>
       </c>
       <c r="F4" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
         <v>12.2837540800199</v>
       </c>
-      <c r="I4" t="n">
-        <v>0.000000000000000000000000000000000664427514046611</v>
+      <c r="I4" s="1">
+        <v>6.6442751404661102E-34</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
-        <v>1.08713453159776</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0173821768274</v>
+      <c r="D5">
+        <v>1.0871345315977601</v>
+      </c>
+      <c r="E5">
+        <v>1.7382176827399998E-2</v>
       </c>
       <c r="F5" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>5.22518276702495</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.000001043899021756</v>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5.2251827670249504</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1.043899021756E-6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>1.07621474818717</v>
       </c>
-      <c r="E6" t="n">
-        <v>0.0240829191418184</v>
+      <c r="E6">
+        <v>2.4082919141818399E-2</v>
       </c>
       <c r="F6" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>3.28232621575695</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.00617726546660551</v>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3.2823262157569499</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6.1772654666055098E-3</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" t="n">
-        <v>0.98995544424981</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.0172046819149167</v>
+      <c r="D7">
+        <v>0.98995544424980997</v>
+      </c>
+      <c r="E7">
+        <v>1.7204681914916701E-2</v>
       </c>
       <c r="F7" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-0.580884871436602</v>
-      </c>
-      <c r="I7" t="n">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-0.58088487143660195</v>
+      </c>
+      <c r="I7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>